<commit_message>
added diversity to the plot.
</commit_message>
<xml_diff>
--- a/01_data/Species list.xlsx
+++ b/01_data/Species list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uqasmi57/Documents/Offline_Projects/rare_reptiles/01_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R\r-projects\Offline_Projects\fire_rare_reptiles\rare_reptiles\01_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E427392B-5F29-654D-8496-6BC827D7CB63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B57416D8-9441-407D-A446-4A2D01879019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="22940" windowHeight="14300" xr2:uid="{D702A044-0976-4545-B026-C759C939EDBD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D702A044-0976-4545-B026-C759C939EDBD}"/>
   </bookViews>
   <sheets>
     <sheet name="Relevant_Species" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="219">
   <si>
     <t>Species Code</t>
   </si>
@@ -546,9 +546,6 @@
   </si>
   <si>
     <t>Abundance</t>
-  </si>
-  <si>
-    <t>Conservation status</t>
   </si>
   <si>
     <t>NA</t>
@@ -1308,25 +1305,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A05311F-4F8B-4906-8B2B-4679EE19E1F6}">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48" customWidth="1"/>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="68.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="68.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18"/>
       <c r="B2" s="19" t="s">
         <v>3</v>
@@ -1338,7 +1335,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F2" s="21" t="s">
         <v>2</v>
@@ -1346,14 +1343,10 @@
       <c r="G2" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="H2" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="I2" s="22" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H2" s="21"/>
+      <c r="I2" s="22"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
       <c r="B3" s="23" t="s">
         <v>7</v>
@@ -1371,14 +1364,10 @@
       <c r="G3" s="24">
         <v>33</v>
       </c>
-      <c r="H3" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="I3" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H3" s="24"/>
+      <c r="I3" s="25"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>51</v>
       </c>
@@ -1396,14 +1385,10 @@
       <c r="G4" s="27">
         <v>92</v>
       </c>
-      <c r="H4" s="27" t="s">
-        <v>77</v>
-      </c>
-      <c r="I4" s="28" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H4" s="27"/>
+      <c r="I4" s="28"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>52</v>
       </c>
@@ -1422,11 +1407,9 @@
         <v>454</v>
       </c>
       <c r="H5" s="27"/>
-      <c r="I5" s="28" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I5" s="28"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>53</v>
       </c>
@@ -1445,11 +1428,9 @@
         <v>5</v>
       </c>
       <c r="H6" s="27"/>
-      <c r="I6" s="28" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I6" s="28"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>54</v>
       </c>
@@ -1470,7 +1451,7 @@
       <c r="H7" s="27"/>
       <c r="I7" s="28"/>
     </row>
-    <row r="8" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18"/>
       <c r="B8" s="29"/>
       <c r="C8" s="30" t="s">
@@ -1486,14 +1467,10 @@
       <c r="G8" s="30">
         <v>1</v>
       </c>
-      <c r="H8" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="I8" s="31" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H8" s="30"/>
+      <c r="I8" s="31"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="18"/>
       <c r="B9" s="23" t="s">
         <v>13</v>
@@ -1511,14 +1488,10 @@
       <c r="G9" s="24">
         <v>1</v>
       </c>
-      <c r="H9" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="I9" s="32" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H9" s="24"/>
+      <c r="I9" s="32"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
       <c r="B10" s="26"/>
       <c r="C10" s="27" t="s">
@@ -1534,14 +1507,10 @@
       <c r="G10" s="27">
         <v>30</v>
       </c>
-      <c r="H10" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="I10" s="28" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H10" s="27"/>
+      <c r="I10" s="28"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
       <c r="B11" s="26"/>
       <c r="C11" s="27" t="s">
@@ -1557,14 +1526,10 @@
       <c r="G11" s="27">
         <v>1</v>
       </c>
-      <c r="H11" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="I11" s="28" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H11" s="27"/>
+      <c r="I11" s="28"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18"/>
       <c r="B12" s="29"/>
       <c r="C12" s="30" t="s">
@@ -1580,14 +1545,10 @@
       <c r="G12" s="11">
         <v>8</v>
       </c>
-      <c r="H12" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="I12" s="31" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H12" s="30"/>
+      <c r="I12" s="31"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="18"/>
       <c r="B13" s="23" t="s">
         <v>18</v>
@@ -1606,11 +1567,9 @@
         <v>42</v>
       </c>
       <c r="H13" s="24"/>
-      <c r="I13" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I13" s="25"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="18"/>
       <c r="B14" s="26"/>
       <c r="C14" s="27" t="s">
@@ -1626,14 +1585,10 @@
       <c r="G14" s="27">
         <v>4</v>
       </c>
-      <c r="H14" s="27" t="s">
-        <v>84</v>
-      </c>
-      <c r="I14" s="28" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H14" s="27"/>
+      <c r="I14" s="28"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
       <c r="B15" s="26"/>
       <c r="C15" s="33" t="s">
@@ -1649,14 +1604,10 @@
       <c r="G15" s="27">
         <v>100</v>
       </c>
-      <c r="H15" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="I15" s="28" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H15" s="27"/>
+      <c r="I15" s="28"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
       <c r="B16" s="26"/>
       <c r="C16" s="27" t="s">
@@ -1673,11 +1624,9 @@
         <v>353</v>
       </c>
       <c r="H16" s="27"/>
-      <c r="I16" s="28" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I16" s="28"/>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="18"/>
       <c r="B17" s="29"/>
       <c r="C17" s="30" t="s">
@@ -1694,11 +1643,9 @@
         <v>6</v>
       </c>
       <c r="H17" s="30"/>
-      <c r="I17" s="31" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I17" s="31"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="18"/>
       <c r="B18" s="23" t="s">
         <v>22</v>
@@ -1716,14 +1663,10 @@
       <c r="G18" s="24">
         <v>22</v>
       </c>
-      <c r="H18" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="I18" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H18" s="24"/>
+      <c r="I18" s="25"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
       <c r="B19" s="26"/>
       <c r="C19" s="27" t="s">
@@ -1739,14 +1682,10 @@
       <c r="G19" s="27">
         <v>7</v>
       </c>
-      <c r="H19" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="I19" s="28" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H19" s="27"/>
+      <c r="I19" s="28"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="18"/>
       <c r="B20" s="26"/>
       <c r="C20" s="27" t="s">
@@ -1763,11 +1702,9 @@
         <v>1</v>
       </c>
       <c r="H20" s="27"/>
-      <c r="I20" s="28" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I20" s="28"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="18"/>
       <c r="B21" s="26"/>
       <c r="C21" s="27" t="s">
@@ -1784,11 +1721,9 @@
         <v>2</v>
       </c>
       <c r="H21" s="27"/>
-      <c r="I21" s="28" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I21" s="28"/>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="18"/>
       <c r="B22" s="26"/>
       <c r="C22" s="27" t="s">
@@ -1805,11 +1740,9 @@
         <v>2</v>
       </c>
       <c r="H22" s="27"/>
-      <c r="I22" s="28" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I22" s="28"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="18"/>
       <c r="B23" s="23" t="s">
         <v>28</v>
@@ -1828,11 +1761,9 @@
         <v>1</v>
       </c>
       <c r="H23" s="24"/>
-      <c r="I23" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I23" s="25"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="18"/>
       <c r="B24" s="26"/>
       <c r="C24" s="27" t="s">
@@ -1848,14 +1779,10 @@
       <c r="G24" s="27">
         <v>73</v>
       </c>
-      <c r="H24" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="I24" s="28" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H24" s="27"/>
+      <c r="I24" s="28"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="18"/>
       <c r="B25" s="26"/>
       <c r="C25" s="27" t="s">
@@ -1872,11 +1799,9 @@
         <v>246</v>
       </c>
       <c r="H25" s="27"/>
-      <c r="I25" s="28" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I25" s="28"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="18"/>
       <c r="B26" s="26"/>
       <c r="C26" s="27" t="s">
@@ -1893,11 +1818,9 @@
         <v>1</v>
       </c>
       <c r="H26" s="27"/>
-      <c r="I26" s="28" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I26" s="28"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="18"/>
       <c r="B27" s="26"/>
       <c r="C27" s="27" t="s">
@@ -1914,11 +1837,9 @@
         <v>125</v>
       </c>
       <c r="H27" s="27"/>
-      <c r="I27" s="28" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I27" s="28"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="18"/>
       <c r="B28" s="26"/>
       <c r="C28" s="27" t="s">
@@ -1935,11 +1856,9 @@
         <v>2</v>
       </c>
       <c r="H28" s="27"/>
-      <c r="I28" s="28" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I28" s="28"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="18"/>
       <c r="B29" s="26"/>
       <c r="C29" s="27" t="s">
@@ -1956,11 +1875,9 @@
         <v>2</v>
       </c>
       <c r="H29" s="27"/>
-      <c r="I29" s="28" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I29" s="28"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="18"/>
       <c r="B30" s="26"/>
       <c r="C30" s="27" t="s">
@@ -1977,11 +1894,9 @@
         <v>50</v>
       </c>
       <c r="H30" s="27"/>
-      <c r="I30" s="28" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I30" s="28"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="18"/>
       <c r="B31" s="26"/>
       <c r="C31" s="27" t="s">
@@ -1998,11 +1913,9 @@
         <v>8</v>
       </c>
       <c r="H31" s="27"/>
-      <c r="I31" s="28" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I31" s="28"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="18"/>
       <c r="B32" s="26"/>
       <c r="C32" s="27" t="s">
@@ -2019,11 +1932,9 @@
         <v>85</v>
       </c>
       <c r="H32" s="27"/>
-      <c r="I32" s="28" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I32" s="28"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="18"/>
       <c r="B33" s="26"/>
       <c r="C33" s="27" t="s">
@@ -2040,11 +1951,9 @@
         <v>24</v>
       </c>
       <c r="H33" s="27"/>
-      <c r="I33" s="28" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I33" s="28"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="18"/>
       <c r="B34" s="26"/>
       <c r="C34" s="27" t="s">
@@ -2061,11 +1970,9 @@
         <v>252</v>
       </c>
       <c r="H34" s="27"/>
-      <c r="I34" s="28" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I34" s="28"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="18"/>
       <c r="B35" s="26"/>
       <c r="C35" s="27" t="s">
@@ -2082,11 +1989,9 @@
         <v>2</v>
       </c>
       <c r="H35" s="27"/>
-      <c r="I35" s="28" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I35" s="28"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="18"/>
       <c r="B36" s="26"/>
       <c r="C36" s="27" t="s">
@@ -2103,11 +2008,9 @@
         <v>2</v>
       </c>
       <c r="H36" s="27"/>
-      <c r="I36" s="28" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I36" s="28"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="18"/>
       <c r="B37" s="26"/>
       <c r="C37" s="27" t="s">
@@ -2124,11 +2027,9 @@
         <v>3</v>
       </c>
       <c r="H37" s="27"/>
-      <c r="I37" s="28" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I37" s="28"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="18"/>
       <c r="B38" s="26"/>
       <c r="C38" s="27" t="s">
@@ -2145,11 +2046,9 @@
         <v>1</v>
       </c>
       <c r="H38" s="27"/>
-      <c r="I38" s="28" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I38" s="28"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="18"/>
       <c r="B39" s="26"/>
       <c r="C39" s="27" t="s">
@@ -2166,11 +2065,9 @@
         <v>24</v>
       </c>
       <c r="H39" s="27"/>
-      <c r="I39" s="28" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I39" s="28"/>
+    </row>
+    <row r="40" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="18"/>
       <c r="B40" s="29"/>
       <c r="C40" s="30" t="s">
@@ -2187,11 +2084,9 @@
         <v>2</v>
       </c>
       <c r="H40" s="30"/>
-      <c r="I40" s="28" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I40" s="28"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="18"/>
       <c r="B41" s="23" t="s">
         <v>47</v>
@@ -2203,7 +2098,7 @@
         <v>141</v>
       </c>
       <c r="E41" s="24" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F41" s="24" t="s">
         <v>109</v>
@@ -2212,11 +2107,9 @@
         <v>15</v>
       </c>
       <c r="H41" s="24"/>
-      <c r="I41" s="28" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I41" s="28"/>
+    </row>
+    <row r="42" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="18"/>
       <c r="B42" s="29"/>
       <c r="C42" s="30" t="s">
@@ -2226,7 +2119,7 @@
         <v>48</v>
       </c>
       <c r="E42" s="30" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F42" s="30" t="s">
         <v>110</v>
@@ -2234,14 +2127,10 @@
       <c r="G42" s="30">
         <v>12</v>
       </c>
-      <c r="H42" s="30" t="s">
-        <v>111</v>
-      </c>
-      <c r="I42" s="28" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H42" s="30"/>
+      <c r="I42" s="28"/>
+    </row>
+    <row r="43" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="18"/>
       <c r="B43" s="19" t="s">
         <v>49</v>
@@ -2260,9 +2149,7 @@
         <v>3</v>
       </c>
       <c r="H43" s="21"/>
-      <c r="I43" s="28" t="s">
-        <v>90</v>
-      </c>
+      <c r="I43" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2278,19 +2165,19 @@
       <selection activeCell="B2" sqref="B2:D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="68.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="68.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="12" t="s">
         <v>3</v>
       </c>
@@ -2317,7 +2204,7 @@
       </c>
       <c r="J2" s="15"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>7</v>
       </c>
@@ -2344,7 +2231,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -2372,7 +2259,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -2398,7 +2285,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -2424,7 +2311,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -2448,7 +2335,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="8"/>
       <c r="C8" s="6" t="s">
         <v>120</v>
@@ -2473,7 +2360,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2500,7 +2387,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
       <c r="C10" s="1" t="s">
         <v>121</v>
@@ -2525,7 +2412,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
       <c r="C11" s="1" t="s">
         <v>135</v>
@@ -2550,7 +2437,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="8"/>
       <c r="C12" s="6" t="s">
         <v>122</v>
@@ -2575,7 +2462,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
         <v>18</v>
       </c>
@@ -2600,7 +2487,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="5"/>
       <c r="C14" s="1" t="s">
         <v>123</v>
@@ -2625,7 +2512,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
       <c r="C15" s="16" t="s">
         <v>114</v>
@@ -2650,7 +2537,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="5"/>
       <c r="C16" s="1" t="s">
         <v>142</v>
@@ -2673,7 +2560,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="8"/>
       <c r="C17" s="6" t="s">
         <v>124</v>
@@ -2696,7 +2583,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
         <v>22</v>
       </c>
@@ -2723,7 +2610,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
       <c r="C19" s="1" t="s">
         <v>125</v>
@@ -2748,7 +2635,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
       <c r="C20" s="1" t="s">
         <v>126</v>
@@ -2771,7 +2658,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
       <c r="C21" s="1" t="s">
         <v>146</v>
@@ -2794,7 +2681,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="5"/>
       <c r="C22" s="1" t="s">
         <v>127</v>
@@ -2817,7 +2704,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="8"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6" t="s">
@@ -2838,7 +2725,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="7" t="s">
         <v>28</v>
       </c>
@@ -2863,7 +2750,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="5"/>
       <c r="C25" s="1" t="s">
         <v>128</v>
@@ -2888,7 +2775,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
       <c r="C26" s="1" t="s">
         <v>129</v>
@@ -2911,7 +2798,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
       <c r="C27" s="1" t="s">
         <v>144</v>
@@ -2934,7 +2821,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="5"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1" t="s">
@@ -2955,7 +2842,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
       <c r="C29" s="1" t="s">
         <v>130</v>
@@ -2978,7 +2865,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="5"/>
       <c r="C30" s="1" t="s">
         <v>131</v>
@@ -3001,7 +2888,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" s="5"/>
       <c r="C31" s="1" t="s">
         <v>132</v>
@@ -3024,7 +2911,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="5"/>
       <c r="C32" s="1" t="s">
         <v>145</v>
@@ -3047,7 +2934,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="5"/>
       <c r="C33" s="1" t="s">
         <v>133</v>
@@ -3070,7 +2957,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" s="5"/>
       <c r="C34" s="1" t="s">
         <v>157</v>
@@ -3093,7 +2980,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" s="5"/>
       <c r="C35" s="1" t="s">
         <v>150</v>
@@ -3116,7 +3003,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36" s="5"/>
       <c r="C36" s="1" t="s">
         <v>147</v>
@@ -3139,7 +3026,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37" s="5"/>
       <c r="C37" s="1" t="s">
         <v>148</v>
@@ -3162,7 +3049,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B38" s="5"/>
       <c r="C38" s="1" t="s">
         <v>151</v>
@@ -3185,7 +3072,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" s="5"/>
       <c r="C39" s="1" t="s">
         <v>152</v>
@@ -3208,7 +3095,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B40" s="5"/>
       <c r="C40" s="1" t="s">
         <v>153</v>
@@ -3231,7 +3118,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41" s="5"/>
       <c r="C41" s="1" t="s">
         <v>154</v>
@@ -3254,7 +3141,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" s="5"/>
       <c r="C42" s="1" t="s">
         <v>155</v>
@@ -3277,7 +3164,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="43" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="8"/>
       <c r="C43" s="6" t="s">
         <v>160</v>
@@ -3300,7 +3187,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44" s="7" t="s">
         <v>47</v>
       </c>
@@ -3325,7 +3212,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="45" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="8"/>
       <c r="C45" s="6" t="s">
         <v>159</v>
@@ -3350,7 +3237,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="46" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="12" t="s">
         <v>49</v>
       </c>
@@ -3385,19 +3272,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE7CCC49-FAE9-494A-94E1-D66FA8360728}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>164</v>
       </c>
@@ -3411,7 +3298,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>113</v>
       </c>
@@ -3425,7 +3312,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>143</v>
       </c>
@@ -3439,7 +3326,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>144</v>
       </c>
@@ -3453,7 +3340,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>126</v>
       </c>
@@ -3467,7 +3354,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>154</v>
       </c>
@@ -3481,7 +3368,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>135</v>
       </c>
@@ -3495,7 +3382,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>120</v>
       </c>
@@ -3509,7 +3396,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>131</v>
       </c>
@@ -3523,7 +3410,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>146</v>
       </c>
@@ -3537,7 +3424,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>148</v>
       </c>
@@ -3551,7 +3438,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>132</v>
       </c>
@@ -3565,7 +3452,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>127</v>
       </c>
@@ -3579,7 +3466,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>151</v>
       </c>
@@ -3593,7 +3480,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>160</v>
       </c>
@@ -3607,7 +3494,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>153</v>
       </c>
@@ -3615,13 +3502,13 @@
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D16" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>156</v>
       </c>
@@ -3629,13 +3516,13 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D17" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>123</v>
       </c>
@@ -3643,13 +3530,13 @@
         <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D18" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>119</v>
       </c>
@@ -3657,13 +3544,13 @@
         <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D19" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>124</v>
       </c>
@@ -3671,13 +3558,13 @@
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D20" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>125</v>
       </c>
@@ -3685,13 +3572,13 @@
         <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D21" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>133</v>
       </c>
@@ -3699,13 +3586,13 @@
         <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D22" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>122</v>
       </c>
@@ -3713,13 +3600,13 @@
         <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D23" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>159</v>
       </c>
@@ -3727,13 +3614,13 @@
         <v>12</v>
       </c>
       <c r="C24" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D24" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>158</v>
       </c>
@@ -3741,13 +3628,13 @@
         <v>15</v>
       </c>
       <c r="C25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D25" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>115</v>
       </c>
@@ -3755,13 +3642,13 @@
         <v>22</v>
       </c>
       <c r="C26" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D26" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>150</v>
       </c>
@@ -3769,13 +3656,13 @@
         <v>24</v>
       </c>
       <c r="C27" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D27" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>155</v>
       </c>
@@ -3783,13 +3670,13 @@
         <v>24</v>
       </c>
       <c r="C28" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D28" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>121</v>
       </c>
@@ -3797,13 +3684,13 @@
         <v>30</v>
       </c>
       <c r="C29" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D29" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>116</v>
       </c>
@@ -3811,13 +3698,13 @@
         <v>33</v>
       </c>
       <c r="C30" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D30" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>134</v>
       </c>
@@ -3825,13 +3712,13 @@
         <v>41</v>
       </c>
       <c r="C31" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D31" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>136</v>
       </c>
@@ -3839,13 +3726,13 @@
         <v>42</v>
       </c>
       <c r="C32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D32" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>145</v>
       </c>
@@ -3853,13 +3740,13 @@
         <v>50</v>
       </c>
       <c r="C33" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D33" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>128</v>
       </c>
@@ -3867,13 +3754,13 @@
         <v>73</v>
       </c>
       <c r="C34" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D34" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>157</v>
       </c>
@@ -3881,13 +3768,13 @@
         <v>85</v>
       </c>
       <c r="C35" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D35" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>117</v>
       </c>
@@ -3895,13 +3782,13 @@
         <v>92</v>
       </c>
       <c r="C36" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D36" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>114</v>
       </c>
@@ -3909,13 +3796,13 @@
         <v>100</v>
       </c>
       <c r="C37" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D37" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>130</v>
       </c>
@@ -3923,13 +3810,13 @@
         <v>125</v>
       </c>
       <c r="C38" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D38" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>129</v>
       </c>
@@ -3937,13 +3824,13 @@
         <v>246</v>
       </c>
       <c r="C39" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D39" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>147</v>
       </c>
@@ -3951,13 +3838,13 @@
         <v>252</v>
       </c>
       <c r="C40" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D40" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>142</v>
       </c>
@@ -3965,13 +3852,13 @@
         <v>353</v>
       </c>
       <c r="C41" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D41" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>118</v>
       </c>
@@ -3979,10 +3866,10 @@
         <v>454</v>
       </c>
       <c r="C42" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D42" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -4001,41 +3888,41 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.6640625" customWidth="1"/>
-    <col min="5" max="5" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>168</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>13</v>
       </c>
@@ -4043,7 +3930,7 @@
         <v>113</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -4058,7 +3945,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>22</v>
       </c>
@@ -4066,7 +3953,7 @@
         <v>115</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D3" s="1">
         <v>22</v>
@@ -4075,13 +3962,13 @@
         <v>90</v>
       </c>
       <c r="F3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G3" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>7</v>
       </c>
@@ -4089,7 +3976,7 @@
         <v>116</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D4" s="1">
         <v>33</v>
@@ -4098,13 +3985,13 @@
         <v>90</v>
       </c>
       <c r="F4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G4" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>13</v>
       </c>
@@ -4112,7 +3999,7 @@
         <v>121</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D5" s="1">
         <v>30</v>
@@ -4121,13 +4008,13 @@
         <v>90</v>
       </c>
       <c r="F5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G5" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>28</v>
       </c>
@@ -4135,7 +4022,7 @@
         <v>128</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D6" s="1">
         <v>73</v>
@@ -4144,13 +4031,13 @@
         <v>90</v>
       </c>
       <c r="F6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G6" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>28</v>
       </c>
@@ -4158,7 +4045,7 @@
         <v>143</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D7" s="6">
         <v>1</v>
@@ -4173,7 +4060,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>7</v>
       </c>
@@ -4181,7 +4068,7 @@
         <v>117</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D8" s="2">
         <v>92</v>
@@ -4190,13 +4077,13 @@
         <v>90</v>
       </c>
       <c r="F8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G8" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>28</v>
       </c>
@@ -4204,7 +4091,7 @@
         <v>129</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D9" s="1">
         <v>246</v>
@@ -4213,13 +4100,13 @@
         <v>90</v>
       </c>
       <c r="F9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G9" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>7</v>
       </c>
@@ -4227,7 +4114,7 @@
         <v>118</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D10" s="1">
         <v>454</v>
@@ -4236,13 +4123,13 @@
         <v>90</v>
       </c>
       <c r="F10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G10" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>28</v>
       </c>
@@ -4250,7 +4137,7 @@
         <v>144</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D11" s="6">
         <v>1</v>
@@ -4265,7 +4152,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>28</v>
       </c>
@@ -4273,7 +4160,7 @@
         <v>131</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D12" s="2">
         <v>2</v>
@@ -4288,7 +4175,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>28</v>
       </c>
@@ -4296,7 +4183,7 @@
         <v>130</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D13" s="1">
         <v>125</v>
@@ -4305,13 +4192,13 @@
         <v>90</v>
       </c>
       <c r="F13" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G13" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>22</v>
       </c>
@@ -4319,7 +4206,7 @@
         <v>125</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D14" s="1">
         <v>7</v>
@@ -4328,13 +4215,13 @@
         <v>89</v>
       </c>
       <c r="F14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G14" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>22</v>
       </c>
@@ -4342,7 +4229,7 @@
         <v>126</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D15" s="1">
         <v>1</v>
@@ -4357,7 +4244,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>18</v>
       </c>
@@ -4365,7 +4252,7 @@
         <v>114</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D16" s="6">
         <v>100</v>
@@ -4374,13 +4261,13 @@
         <v>90</v>
       </c>
       <c r="F16" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G16" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>22</v>
       </c>
@@ -4388,7 +4275,7 @@
         <v>146</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D17" s="2">
         <v>2</v>
@@ -4403,7 +4290,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>18</v>
       </c>
@@ -4411,7 +4298,7 @@
         <v>136</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D18" s="1">
         <v>42</v>
@@ -4420,13 +4307,13 @@
         <v>90</v>
       </c>
       <c r="F18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G18" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>28</v>
       </c>
@@ -4434,7 +4321,7 @@
         <v>147</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D19" s="1">
         <v>252</v>
@@ -4443,13 +4330,13 @@
         <v>90</v>
       </c>
       <c r="F19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G19" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>28</v>
       </c>
@@ -4457,7 +4344,7 @@
         <v>148</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D20" s="1">
         <v>2</v>
@@ -4472,7 +4359,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>18</v>
       </c>
@@ -4480,7 +4367,7 @@
         <v>123</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D21" s="1">
         <v>4</v>
@@ -4489,13 +4376,13 @@
         <v>90</v>
       </c>
       <c r="F21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G21" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>28</v>
       </c>
@@ -4503,7 +4390,7 @@
         <v>132</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D22" s="2">
         <v>2</v>
@@ -4518,7 +4405,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>22</v>
       </c>
@@ -4526,7 +4413,7 @@
         <v>127</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D23" s="1">
         <v>2</v>
@@ -4541,7 +4428,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>28</v>
       </c>
@@ -4549,7 +4436,7 @@
         <v>145</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D24" s="1">
         <v>50</v>
@@ -4558,13 +4445,13 @@
         <v>90</v>
       </c>
       <c r="F24" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G24" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>28</v>
       </c>
@@ -4572,7 +4459,7 @@
         <v>133</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D25" s="1">
         <v>8</v>
@@ -4581,13 +4468,13 @@
         <v>90</v>
       </c>
       <c r="F25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G25" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>28</v>
       </c>
@@ -4595,7 +4482,7 @@
         <v>157</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D26" s="1">
         <v>85</v>
@@ -4604,13 +4491,13 @@
         <v>90</v>
       </c>
       <c r="F26" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G26" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>28</v>
       </c>
@@ -4618,7 +4505,7 @@
         <v>150</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D27" s="1">
         <v>24</v>
@@ -4627,13 +4514,13 @@
         <v>90</v>
       </c>
       <c r="F27" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G27" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
         <v>28</v>
       </c>
@@ -4641,7 +4528,7 @@
         <v>153</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D28" s="1">
         <v>3</v>
@@ -4650,13 +4537,13 @@
         <v>90</v>
       </c>
       <c r="F28" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G28" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
         <v>28</v>
       </c>
@@ -4664,7 +4551,7 @@
         <v>154</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D29" s="1">
         <v>1</v>
@@ -4679,7 +4566,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>28</v>
       </c>
@@ -4687,7 +4574,7 @@
         <v>151</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D30" s="1">
         <v>2</v>
@@ -4702,7 +4589,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>7</v>
       </c>
@@ -4710,7 +4597,7 @@
         <v>119</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D31" s="1">
         <v>5</v>
@@ -4719,13 +4606,13 @@
         <v>90</v>
       </c>
       <c r="F31" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G31" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
         <v>28</v>
       </c>
@@ -4733,7 +4620,7 @@
         <v>155</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D32" s="1">
         <v>24</v>
@@ -4742,13 +4629,13 @@
         <v>90</v>
       </c>
       <c r="F32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G32" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>18</v>
       </c>
@@ -4756,7 +4643,7 @@
         <v>142</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D33" s="1">
         <v>353</v>
@@ -4765,13 +4652,13 @@
         <v>90</v>
       </c>
       <c r="F33" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G33" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>13</v>
       </c>
@@ -4779,7 +4666,7 @@
         <v>135</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D34" s="1">
         <v>1</v>
@@ -4794,7 +4681,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>7</v>
       </c>
@@ -4802,22 +4689,22 @@
         <v>134</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D35" s="1">
         <v>41</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F35" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G35" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
         <v>47</v>
       </c>
@@ -4825,7 +4712,7 @@
         <v>158</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D36" s="1">
         <v>15</v>
@@ -4834,13 +4721,13 @@
         <v>90</v>
       </c>
       <c r="F36" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G36" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
         <v>47</v>
       </c>
@@ -4848,7 +4735,7 @@
         <v>159</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D37" s="1">
         <v>12</v>
@@ -4857,13 +4744,13 @@
         <v>90</v>
       </c>
       <c r="F37" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G37" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
         <v>18</v>
       </c>
@@ -4871,7 +4758,7 @@
         <v>124</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D38" s="1">
         <v>6</v>
@@ -4880,13 +4767,13 @@
         <v>90</v>
       </c>
       <c r="F38" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G38" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>13</v>
       </c>
@@ -4894,7 +4781,7 @@
         <v>122</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D39" s="11">
         <v>8</v>
@@ -4903,13 +4790,13 @@
         <v>90</v>
       </c>
       <c r="F39" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G39" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>7</v>
       </c>
@@ -4917,7 +4804,7 @@
         <v>120</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D40" s="2">
         <v>1</v>
@@ -4932,7 +4819,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>28</v>
       </c>
@@ -4940,7 +4827,7 @@
         <v>160</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D41" s="6">
         <v>2</v>
@@ -4955,7 +4842,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="12" t="s">
         <v>49</v>
       </c>
@@ -4963,7 +4850,7 @@
         <v>156</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D42" s="14">
         <v>3</v>
@@ -4972,7 +4859,7 @@
         <v>90</v>
       </c>
       <c r="F42" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G42" t="s">
         <v>165</v>

</xml_diff>